<commit_message>
Fim do semestre 2018-2 (do jeito que estão, sem revisão)
Códigos-fonte em que trabalhamos em sala de aula neste semestre (do jeito que estão, sem revisão)
</commit_message>
<xml_diff>
--- a/data/D01_Iris.xlsx
+++ b/data/D01_Iris.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_GitHub\EEL891\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D47975EA-E25D-414E-9ACB-61BCBA51332D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -28,14 +34,14 @@
     <t>petal width (cm)</t>
   </si>
   <si>
-    <t>target</t>
+    <t>alvo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,11 +104,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -144,7 +158,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -176,9 +190,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -210,6 +242,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -385,14 +435,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F151"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G95" sqref="G95"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -409,12 +470,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>5.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="C2">
         <v>3.5</v>
@@ -429,12 +490,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="C3">
         <v>3</v>
@@ -449,7 +510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -469,12 +530,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="C5">
         <v>3.1</v>
@@ -489,7 +550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -509,7 +570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -529,12 +590,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="C8">
         <v>3.4</v>
@@ -549,7 +610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -569,12 +630,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C10">
         <v>2.9</v>
@@ -589,12 +650,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="C11">
         <v>3.1</v>
@@ -609,7 +670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -629,7 +690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -649,7 +710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -669,7 +730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -680,7 +741,7 @@
         <v>3</v>
       </c>
       <c r="D15">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="E15">
         <v>0.1</v>
@@ -689,7 +750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -709,7 +770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -717,7 +778,7 @@
         <v>5.7</v>
       </c>
       <c r="C17">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="D17">
         <v>1.5</v>
@@ -729,7 +790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -749,12 +810,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19">
-        <v>5.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="C19">
         <v>3.5</v>
@@ -769,7 +830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -789,12 +850,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21">
-        <v>5.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="C21">
         <v>3.8</v>
@@ -809,7 +870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -829,12 +890,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23">
-        <v>5.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="C23">
         <v>3.7</v>
@@ -849,12 +910,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="C24">
         <v>3.6</v>
@@ -869,12 +930,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25">
-        <v>5.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="C25">
         <v>3.3</v>
@@ -889,7 +950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -909,7 +970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -929,7 +990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -949,7 +1010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -969,7 +1030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -989,7 +1050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1009,7 +1070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1029,7 +1090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1049,7 +1110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1057,7 +1118,7 @@
         <v>5.2</v>
       </c>
       <c r="C34">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="D34">
         <v>1.5</v>
@@ -1069,7 +1130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1089,12 +1150,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>34</v>
       </c>
       <c r="B36">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="C36">
         <v>3.1</v>
@@ -1109,7 +1170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1129,7 +1190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1149,12 +1210,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
       <c r="B39">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="C39">
         <v>3.1</v>
@@ -1169,12 +1230,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
       <c r="B40">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C40">
         <v>3</v>
@@ -1189,12 +1250,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>39</v>
       </c>
       <c r="B41">
-        <v>5.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="C41">
         <v>3.4</v>
@@ -1209,7 +1270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -1229,7 +1290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -1237,7 +1298,7 @@
         <v>4.5</v>
       </c>
       <c r="C43">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="D43">
         <v>1.3</v>
@@ -1249,12 +1310,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42</v>
       </c>
       <c r="B44">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C44">
         <v>3.2</v>
@@ -1269,7 +1330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -1289,12 +1350,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44</v>
       </c>
       <c r="B46">
-        <v>5.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="C46">
         <v>3.8</v>
@@ -1309,7 +1370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -1329,12 +1390,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>46</v>
       </c>
       <c r="B48">
-        <v>5.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="C48">
         <v>3.8</v>
@@ -1349,12 +1410,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>47</v>
       </c>
       <c r="B49">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="C49">
         <v>3.2</v>
@@ -1369,7 +1430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -1389,7 +1450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -1409,7 +1470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -1429,7 +1490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -1449,7 +1510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -1460,7 +1521,7 @@
         <v>3.1</v>
       </c>
       <c r="D54">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="E54">
         <v>1.5</v>
@@ -1469,7 +1530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -1477,7 +1538,7 @@
         <v>5.5</v>
       </c>
       <c r="C55">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="D55">
         <v>4</v>
@@ -1489,7 +1550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -1500,7 +1561,7 @@
         <v>2.8</v>
       </c>
       <c r="D56">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="E56">
         <v>1.5</v>
@@ -1509,7 +1570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -1529,7 +1590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -1549,12 +1610,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>57</v>
       </c>
       <c r="B59">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="C59">
         <v>2.4</v>
@@ -1569,7 +1630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -1580,7 +1641,7 @@
         <v>2.9</v>
       </c>
       <c r="D60">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="E60">
         <v>1.3</v>
@@ -1589,7 +1650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -1609,7 +1670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -1629,7 +1690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -1649,7 +1710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -1657,7 +1718,7 @@
         <v>6</v>
       </c>
       <c r="C64">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D64">
         <v>4</v>
@@ -1669,7 +1730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -1689,7 +1750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -1709,7 +1770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -1720,7 +1781,7 @@
         <v>3.1</v>
       </c>
       <c r="D67">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="E67">
         <v>1.4</v>
@@ -1729,7 +1790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -1749,7 +1810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -1760,7 +1821,7 @@
         <v>2.7</v>
       </c>
       <c r="D69">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="E69">
         <v>1</v>
@@ -1769,7 +1830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -1777,7 +1838,7 @@
         <v>6.2</v>
       </c>
       <c r="C70">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D70">
         <v>4.5</v>
@@ -1789,7 +1850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -1803,13 +1864,13 @@
         <v>3.9</v>
       </c>
       <c r="E71">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F71">
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:6">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -1829,7 +1890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -1849,7 +1910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:6">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -1860,7 +1921,7 @@
         <v>2.5</v>
       </c>
       <c r="D74">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="E74">
         <v>1.5</v>
@@ -1869,7 +1930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -1889,7 +1950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:6">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -1909,7 +1970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:6">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -1920,7 +1981,7 @@
         <v>3</v>
       </c>
       <c r="D77">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="E77">
         <v>1.4</v>
@@ -1929,7 +1990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:6">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -1949,7 +2010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -1969,7 +2030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:6">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -1989,7 +2050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -2009,7 +2070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -2023,13 +2084,13 @@
         <v>3.8</v>
       </c>
       <c r="E82">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F82">
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -2049,7 +2110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -2069,7 +2130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -2080,7 +2141,7 @@
         <v>2.7</v>
       </c>
       <c r="D85">
-        <v>5.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="E85">
         <v>1.6</v>
@@ -2089,7 +2150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -2109,7 +2170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -2129,7 +2190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -2149,7 +2210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -2157,10 +2218,10 @@
         <v>6.3</v>
       </c>
       <c r="C89">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="D89">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="E89">
         <v>1.3</v>
@@ -2169,7 +2230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -2180,7 +2241,7 @@
         <v>3</v>
       </c>
       <c r="D90">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="E90">
         <v>1.3</v>
@@ -2189,7 +2250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -2209,7 +2270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -2220,7 +2281,7 @@
         <v>2.6</v>
       </c>
       <c r="D92">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="E92">
         <v>1.2</v>
@@ -2229,7 +2290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -2240,7 +2301,7 @@
         <v>3</v>
       </c>
       <c r="D93">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="E93">
         <v>1.4</v>
@@ -2249,7 +2310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -2269,7 +2330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:6">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -2277,7 +2338,7 @@
         <v>5</v>
       </c>
       <c r="C95">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="D95">
         <v>3.3</v>
@@ -2289,7 +2350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -2309,7 +2370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:6">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -2329,7 +2390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:6">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -2349,7 +2410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:6">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -2369,12 +2430,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:6">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>98</v>
       </c>
       <c r="B100">
-        <v>5.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="C100">
         <v>2.5</v>
@@ -2383,13 +2444,13 @@
         <v>3</v>
       </c>
       <c r="E100">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F100">
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:6">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -2400,7 +2461,7 @@
         <v>2.8</v>
       </c>
       <c r="D101">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="E101">
         <v>1.3</v>
@@ -2409,7 +2470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:6">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -2429,7 +2490,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="103" spans="1:6">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -2440,7 +2501,7 @@
         <v>2.7</v>
       </c>
       <c r="D103">
-        <v>5.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="E103">
         <v>1.9</v>
@@ -2449,7 +2510,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="1:6">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -2469,7 +2530,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="1:6">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -2489,7 +2550,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="106" spans="1:6">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -2503,13 +2564,13 @@
         <v>5.8</v>
       </c>
       <c r="E106">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F106">
         <v>2</v>
       </c>
     </row>
-    <row r="107" spans="1:6">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -2529,12 +2590,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="1:6">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>106</v>
       </c>
       <c r="B108">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="C108">
         <v>2.5</v>
@@ -2549,7 +2610,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="109" spans="1:6">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -2569,7 +2630,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="110" spans="1:6">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -2589,7 +2650,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="111" spans="1:6">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -2609,7 +2670,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="112" spans="1:6">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -2620,7 +2681,7 @@
         <v>3.2</v>
       </c>
       <c r="D112">
-        <v>5.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="E112">
         <v>2</v>
@@ -2629,7 +2690,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="113" spans="1:6">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -2649,7 +2710,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="114" spans="1:6">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -2669,7 +2730,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="115" spans="1:6">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -2689,7 +2750,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="116" spans="1:6">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -2700,7 +2761,7 @@
         <v>2.8</v>
       </c>
       <c r="D116">
-        <v>5.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="E116">
         <v>2.4</v>
@@ -2709,7 +2770,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="117" spans="1:6">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -2723,13 +2784,13 @@
         <v>5.3</v>
       </c>
       <c r="E117">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="F117">
         <v>2</v>
       </c>
     </row>
-    <row r="118" spans="1:6">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -2749,7 +2810,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="119" spans="1:6">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -2763,13 +2824,13 @@
         <v>6.7</v>
       </c>
       <c r="E119">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F119">
         <v>2</v>
       </c>
     </row>
-    <row r="120" spans="1:6">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -2783,13 +2844,13 @@
         <v>6.9</v>
       </c>
       <c r="E120">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="F120">
         <v>2</v>
       </c>
     </row>
-    <row r="121" spans="1:6">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -2797,7 +2858,7 @@
         <v>6</v>
       </c>
       <c r="C121">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D121">
         <v>5</v>
@@ -2809,7 +2870,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="122" spans="1:6">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>120</v>
       </c>
@@ -2823,13 +2884,13 @@
         <v>5.7</v>
       </c>
       <c r="E122">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="F122">
         <v>2</v>
       </c>
     </row>
-    <row r="123" spans="1:6">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>121</v>
       </c>
@@ -2840,7 +2901,7 @@
         <v>2.8</v>
       </c>
       <c r="D123">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="E123">
         <v>2</v>
@@ -2849,7 +2910,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="124" spans="1:6">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>122</v>
       </c>
@@ -2869,7 +2930,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="125" spans="1:6">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>123</v>
       </c>
@@ -2880,7 +2941,7 @@
         <v>2.7</v>
       </c>
       <c r="D125">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="E125">
         <v>1.8</v>
@@ -2889,7 +2950,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="126" spans="1:6">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>124</v>
       </c>
@@ -2909,7 +2970,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="127" spans="1:6">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>125</v>
       </c>
@@ -2929,7 +2990,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="128" spans="1:6">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>126</v>
       </c>
@@ -2949,7 +3010,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="129" spans="1:6">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -2960,7 +3021,7 @@
         <v>3</v>
       </c>
       <c r="D129">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="E129">
         <v>1.8</v>
@@ -2969,7 +3030,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="130" spans="1:6">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -2989,7 +3050,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="131" spans="1:6">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>129</v>
       </c>
@@ -3009,7 +3070,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="132" spans="1:6">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>130</v>
       </c>
@@ -3029,7 +3090,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="133" spans="1:6">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -3049,7 +3110,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="134" spans="1:6">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>132</v>
       </c>
@@ -3063,13 +3124,13 @@
         <v>5.6</v>
       </c>
       <c r="E134">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F134">
         <v>2</v>
       </c>
     </row>
-    <row r="135" spans="1:6">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>133</v>
       </c>
@@ -3080,7 +3141,7 @@
         <v>2.8</v>
       </c>
       <c r="D135">
-        <v>5.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="E135">
         <v>1.5</v>
@@ -3089,7 +3150,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="136" spans="1:6">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -3109,7 +3170,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="137" spans="1:6">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -3123,13 +3184,13 @@
         <v>6.1</v>
       </c>
       <c r="E137">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="F137">
         <v>2</v>
       </c>
     </row>
-    <row r="138" spans="1:6">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>136</v>
       </c>
@@ -3149,7 +3210,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="139" spans="1:6">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>137</v>
       </c>
@@ -3169,7 +3230,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="140" spans="1:6">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>138</v>
       </c>
@@ -3189,7 +3250,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="141" spans="1:6">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>139</v>
       </c>
@@ -3209,7 +3270,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="142" spans="1:6">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>140</v>
       </c>
@@ -3229,7 +3290,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="143" spans="1:6">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>141</v>
       </c>
@@ -3240,16 +3301,16 @@
         <v>3.1</v>
       </c>
       <c r="D143">
-        <v>5.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="E143">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="F143">
         <v>2</v>
       </c>
     </row>
-    <row r="144" spans="1:6">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>142</v>
       </c>
@@ -3260,7 +3321,7 @@
         <v>2.7</v>
       </c>
       <c r="D144">
-        <v>5.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="E144">
         <v>1.9</v>
@@ -3269,7 +3330,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="145" spans="1:6">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>143</v>
       </c>
@@ -3283,13 +3344,13 @@
         <v>5.9</v>
       </c>
       <c r="E145">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="F145">
         <v>2</v>
       </c>
     </row>
-    <row r="146" spans="1:6">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>144</v>
       </c>
@@ -3309,7 +3370,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="147" spans="1:6">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>145</v>
       </c>
@@ -3323,13 +3384,13 @@
         <v>5.2</v>
       </c>
       <c r="E147">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="F147">
         <v>2</v>
       </c>
     </row>
-    <row r="148" spans="1:6">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>146</v>
       </c>
@@ -3349,7 +3410,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="149" spans="1:6">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>147</v>
       </c>
@@ -3369,7 +3430,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="150" spans="1:6">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>148</v>
       </c>
@@ -3383,13 +3444,13 @@
         <v>5.4</v>
       </c>
       <c r="E150">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="F150">
         <v>2</v>
       </c>
     </row>
-    <row r="151" spans="1:6">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>149</v>
       </c>
@@ -3400,7 +3461,7 @@
         <v>3</v>
       </c>
       <c r="D151">
-        <v>5.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="E151">
         <v>1.8</v>

</xml_diff>